<commit_message>
Getting probability distributions working
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63470579-17A4-48A2-8177-D59EB39875AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449BC65C-96DF-4AE3-9F65-EA84375A6433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25980" yWindow="2115" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -710,7 +710,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1140,7 @@
         <v>236</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="G26" t="s">
         <v>90</v>
@@ -1342,7 +1342,7 @@
         <v>503.82</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G36" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Fitting probability distribution to results and plotting
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449BC65C-96DF-4AE3-9F65-EA84375A6433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30B597B-4219-49B2-A25F-4724CE554874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -279,12 +279,6 @@
     <t>% pipe diameter (m)</t>
   </si>
   <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>% Young's modulus (GPa)</t>
-  </si>
-  <si>
     <t>LE (5%, or min when using Uniform distribution)</t>
   </si>
   <si>
@@ -340,6 +334,12 @@
   </si>
   <si>
     <t>Parameter</t>
+  </si>
+  <si>
+    <t>EI</t>
+  </si>
+  <si>
+    <t>% pipe bending stiffness (kNm2)</t>
   </si>
 </sst>
 </file>
@@ -747,7 +747,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -777,12 +777,12 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,29 +872,29 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -924,7 +924,13 @@
         <v>13</v>
       </c>
       <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>10</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
       </c>
       <c r="G12" t="s">
         <v>22</v>
@@ -954,13 +960,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="G15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -970,16 +976,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>33</v>
@@ -1108,22 +1114,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B25">
-        <v>210</v>
+        <v>61675</v>
       </c>
       <c r="C25">
-        <v>210</v>
+        <v>61675</v>
       </c>
       <c r="D25">
-        <v>210</v>
+        <v>61675</v>
       </c>
       <c r="E25" t="s">
         <v>76</v>
       </c>
       <c r="G25" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1143,7 +1149,7 @@
         <v>75</v>
       </c>
       <c r="G26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1465,7 +1471,7 @@
         <v>34</v>
       </c>
       <c r="G42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1485,12 +1491,12 @@
         <v>76</v>
       </c>
       <c r="G43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B44" s="3">
         <v>26.6</v>
@@ -1505,7 +1511,7 @@
         <v>34</v>
       </c>
       <c r="G44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Making error consistent, running a couple of examples to check impact
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCE0153-65FC-47D3-AB45-E81B34254881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54594FF9-4C0A-4BE7-9217-05BCB8E53AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -463,6 +463,1071 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114813</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="43" name="Group 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9EAD8BA-9958-45B9-A45A-E045D1BBA7E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4552950" y="2286000"/>
+          <a:ext cx="4781550" cy="3162813"/>
+          <a:chOff x="5772151" y="1085850"/>
+          <a:chExt cx="4781550" cy="3162813"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="44" name="Picture 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67139CBB-AC16-4A1D-1075-DD3D57FEA0C1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect t="13987" r="49197"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5772151" y="1085850"/>
+            <a:ext cx="4781550" cy="3162813"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="45" name="Straight Connector 44">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{230F3240-0B9C-248D-4363-936E978C10E4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7115175" y="2124075"/>
+            <a:ext cx="0" cy="1638300"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="46" name="Cross 45">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36438FC0-4EDD-DB43-D637-2B20E453EA75}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="2685931">
+            <a:off x="7058706" y="2071689"/>
+            <a:ext cx="108000" cy="108000"/>
+          </a:xfrm>
+          <a:prstGeom prst="plus">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 41479"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-AU" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="47" name="Straight Connector 46">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B83E45F-2B1E-C24D-EC0F-1C9D6BA4C6E3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="6341175" y="2133538"/>
+            <a:ext cx="775980" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="48" name="TextBox 47">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B7DC353-9222-8B90-3FD8-1EA4452CAEE2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5962649" y="2006435"/>
+            <a:ext cx="434734" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>0.72</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76711</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="49" name="Group 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F633030A-8F6A-45D7-83FE-ED399179A4CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9429750" y="2286000"/>
+          <a:ext cx="4724400" cy="3124711"/>
+          <a:chOff x="5772150" y="5105400"/>
+          <a:chExt cx="4724400" cy="3124711"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="50" name="Picture 49">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA5C477F-7AFF-85BB-5F57-B080F1916555}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:srcRect t="14581" r="49956"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5772150" y="5105400"/>
+            <a:ext cx="4724400" cy="3124711"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="51" name="Straight Connector 50">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2835A5B4-B7B6-8EEF-4E9F-B39214ED9200}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7791613" y="6149064"/>
+            <a:ext cx="0" cy="1591200"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="52" name="Cross 51">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4439168-7CF7-06B0-6019-46BDC8FB78F8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="2685931">
+            <a:off x="7735144" y="6096678"/>
+            <a:ext cx="108000" cy="108000"/>
+          </a:xfrm>
+          <a:prstGeom prst="plus">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 41479"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-AU" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="53" name="Straight Connector 52">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA8ACF7B-A12A-6684-3CF2-D96334C5820D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="6356351" y="6152069"/>
+            <a:ext cx="1420063" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="54" name="TextBox 53">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74FF9D5F-966E-8655-C1AC-25BC4A42400A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5977826" y="6024966"/>
+            <a:ext cx="434734" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>0.72</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="55" name="Straight Connector 54">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9870770D-B10A-02E6-D1F9-82C4173C9B9F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="6360225" y="5933155"/>
+            <a:ext cx="1762063" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="56" name="Straight Connector 55">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51B51D32-1B2E-F121-5350-A34B131D44E1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="6360871" y="6366461"/>
+            <a:ext cx="1168709" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="57" name="TextBox 56">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F41E8623-0DF5-9E4A-71CA-0BB2E8CFB571}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6410489" y="5906145"/>
+            <a:ext cx="429028" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>+X%</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="58" name="TextBox 57">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B32863E0-ED35-99C8-25D6-7739C1E6B217}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6433412" y="6125060"/>
+            <a:ext cx="401970" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>-X%</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="59" name="Straight Connector 58">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDBE68AF-18B1-4BE9-317E-A8C5798475C8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7531371" y="6366041"/>
+            <a:ext cx="0" cy="1368000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="60" name="Straight Connector 59">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08637ED1-6799-4CA3-FAF1-37F55DE786EA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8128701" y="5934026"/>
+            <a:ext cx="0" cy="1800000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="61" name="Cross 60">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48454CC4-DB7F-CCAA-8993-C79FA0F0D7C1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="2685931">
+            <a:off x="7478131" y="6316884"/>
+            <a:ext cx="108000" cy="108000"/>
+          </a:xfrm>
+          <a:prstGeom prst="plus">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 41479"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-AU" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="62" name="Cross 61">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34481FBE-04E5-E6C6-0951-89B23180C582}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="2685931">
+            <a:off x="8075462" y="5878411"/>
+            <a:ext cx="108000" cy="108000"/>
+          </a:xfrm>
+          <a:prstGeom prst="plus">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 41479"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-AU" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="63" name="Straight Arrow Connector 62">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECAA3A46-5DC7-1958-C1BE-9330832837BF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="6418373" y="5928101"/>
+            <a:ext cx="0" cy="216000"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:headEnd type="triangle"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="64" name="Straight Arrow Connector 63">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FB6387B-4422-27B1-6C7B-CD33847A908E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="6415790" y="6154764"/>
+            <a:ext cx="0" cy="216000"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:headEnd type="triangle"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="65" name="Straight Arrow Connector 64">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0554B80B-6F70-C071-2C15-07DDA464B1A3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="7532959" y="7663164"/>
+            <a:ext cx="591059" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:headEnd type="triangle"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="66" name="TextBox 65">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5E52E92-580C-420E-8836-21C3EE3855D7}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7768849" y="7403669"/>
+            <a:ext cx="2051652" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-AU" sz="1100">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Range of allowed random values</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -849,7 +1914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1687,10 +2752,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB89FDF4-C5C2-405B-8802-1B03DEB1F621}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,7 +2766,7 @@
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>104</v>
       </c>
@@ -1712,7 +2777,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1721,7 +2786,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1730,7 +2795,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1739,7 +2804,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1748,7 +2813,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1757,7 +2822,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1766,7 +2831,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -1775,7 +2840,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1784,7 +2849,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1793,7 +2858,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1802,7 +2867,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1811,7 +2876,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1819,8 +2884,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1835,7 +2901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -1850,7 +2916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2020,6 +3086,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Setting up data correlation taking parts from mcerp
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54594FF9-4C0A-4BE7-9217-05BCB8E53AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACC909F-7DE8-40AD-B68C-322EB2A52732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="110">
   <si>
     <t>Input File for Pipe-Soil Interaction Analysis</t>
   </si>
@@ -352,36 +352,22 @@
     <t>Min Value</t>
   </si>
   <si>
-    <t>Correlated to:</t>
-  </si>
-  <si>
-    <t>Strongly or Weakly?</t>
-  </si>
-  <si>
-    <t>Strongly</t>
-  </si>
-  <si>
-    <t>Weakly</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">±% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Window</t>
-    </r>
+    <t>Correlation Index</t>
+  </si>
+  <si>
+    <t>Strongly Positive</t>
+  </si>
+  <si>
+    <t>Weakly Positive</t>
+  </si>
+  <si>
+    <t>Weakly Negative</t>
+  </si>
+  <si>
+    <t>Correlation Type</t>
+  </si>
+  <si>
+    <t>Base Variable</t>
   </si>
 </sst>
 </file>
@@ -392,7 +378,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,15 +395,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -463,1071 +444,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>114813</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="43" name="Group 42">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9EAD8BA-9958-45B9-A45A-E045D1BBA7E1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="4552950" y="2286000"/>
-          <a:ext cx="4781550" cy="3162813"/>
-          <a:chOff x="5772151" y="1085850"/>
-          <a:chExt cx="4781550" cy="3162813"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="44" name="Picture 43">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67139CBB-AC16-4A1D-1075-DD3D57FEA0C1}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-          <a:srcRect t="13987" r="49197"/>
-          <a:stretch/>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5772151" y="1085850"/>
-            <a:ext cx="4781550" cy="3162813"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="45" name="Straight Connector 44">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{230F3240-0B9C-248D-4363-936E978C10E4}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7115175" y="2124075"/>
-            <a:ext cx="0" cy="1638300"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="38100">
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="46" name="Cross 45">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36438FC0-4EDD-DB43-D637-2B20E453EA75}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="2685931">
-            <a:off x="7058706" y="2071689"/>
-            <a:ext cx="108000" cy="108000"/>
-          </a:xfrm>
-          <a:prstGeom prst="plus">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 41479"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="00B050"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-AU" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="47" name="Straight Connector 46">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B83E45F-2B1E-C24D-EC0F-1C9D6BA4C6E3}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="6341175" y="2133538"/>
-            <a:ext cx="775980" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="38100">
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="48" name="TextBox 47">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B7DC353-9222-8B90-3FD8-1EA4452CAEE2}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5962649" y="2006435"/>
-            <a:ext cx="434734" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1100">
-                <a:solidFill>
-                  <a:srgbClr val="00B050"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>0.72</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>76711</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="49" name="Group 48">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F633030A-8F6A-45D7-83FE-ED399179A4CB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="9429750" y="2286000"/>
-          <a:ext cx="4724400" cy="3124711"/>
-          <a:chOff x="5772150" y="5105400"/>
-          <a:chExt cx="4724400" cy="3124711"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="50" name="Picture 49">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA5C477F-7AFF-85BB-5F57-B080F1916555}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-          <a:srcRect t="14581" r="49956"/>
-          <a:stretch/>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5772150" y="5105400"/>
-            <a:ext cx="4724400" cy="3124711"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="51" name="Straight Connector 50">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2835A5B4-B7B6-8EEF-4E9F-B39214ED9200}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7791613" y="6149064"/>
-            <a:ext cx="0" cy="1591200"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="38100">
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="52" name="Cross 51">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4439168-7CF7-06B0-6019-46BDC8FB78F8}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="2685931">
-            <a:off x="7735144" y="6096678"/>
-            <a:ext cx="108000" cy="108000"/>
-          </a:xfrm>
-          <a:prstGeom prst="plus">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 41479"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="00B050"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-AU" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="53" name="Straight Connector 52">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA8ACF7B-A12A-6684-3CF2-D96334C5820D}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="6356351" y="6152069"/>
-            <a:ext cx="1420063" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="38100">
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="54" name="TextBox 53">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74FF9D5F-966E-8655-C1AC-25BC4A42400A}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5977826" y="6024966"/>
-            <a:ext cx="434734" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1100">
-                <a:solidFill>
-                  <a:srgbClr val="00B050"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>0.72</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="55" name="Straight Connector 54">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9870770D-B10A-02E6-D1F9-82C4173C9B9F}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="6360225" y="5933155"/>
-            <a:ext cx="1762063" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="38100">
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="56" name="Straight Connector 55">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51B51D32-1B2E-F121-5350-A34B131D44E1}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipV="1">
-            <a:off x="6360871" y="6366461"/>
-            <a:ext cx="1168709" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="38100">
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="57" name="TextBox 56">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F41E8623-0DF5-9E4A-71CA-0BB2E8CFB571}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6410489" y="5906145"/>
-            <a:ext cx="429028" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1100">
-                <a:solidFill>
-                  <a:srgbClr val="00B050"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>+X%</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="58" name="TextBox 57">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B32863E0-ED35-99C8-25D6-7739C1E6B217}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="6433412" y="6125060"/>
-            <a:ext cx="401970" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1100">
-                <a:solidFill>
-                  <a:srgbClr val="00B050"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>-X%</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="59" name="Straight Connector 58">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDBE68AF-18B1-4BE9-317E-A8C5798475C8}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7531371" y="6366041"/>
-            <a:ext cx="0" cy="1368000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="38100">
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="60" name="Straight Connector 59">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08637ED1-6799-4CA3-FAF1-37F55DE786EA}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8128701" y="5934026"/>
-            <a:ext cx="0" cy="1800000"/>
-          </a:xfrm>
-          <a:prstGeom prst="line">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln w="38100">
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="61" name="Cross 60">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48454CC4-DB7F-CCAA-8993-C79FA0F0D7C1}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="2685931">
-            <a:off x="7478131" y="6316884"/>
-            <a:ext cx="108000" cy="108000"/>
-          </a:xfrm>
-          <a:prstGeom prst="plus">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 41479"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="FFC000"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-AU" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="62" name="Cross 61">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34481FBE-04E5-E6C6-0951-89B23180C582}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="2685931">
-            <a:off x="8075462" y="5878411"/>
-            <a:ext cx="108000" cy="108000"/>
-          </a:xfrm>
-          <a:prstGeom prst="plus">
-            <a:avLst>
-              <a:gd name="adj" fmla="val 41479"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="FFC000"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="15000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-AU" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="63" name="Straight Arrow Connector 62">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECAA3A46-5DC7-1958-C1BE-9330832837BF}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="6418373" y="5928101"/>
-            <a:ext cx="0" cy="216000"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:headEnd type="triangle"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="64" name="Straight Arrow Connector 63">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FB6387B-4422-27B1-6C7B-CD33847A908E}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1">
-            <a:off x="6415790" y="6154764"/>
-            <a:ext cx="0" cy="216000"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:headEnd type="triangle"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:cxnSp macro="">
-        <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="65" name="Straight Arrow Connector 64">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0554B80B-6F70-C071-2C15-07DDA464B1A3}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvCxnSpPr/>
-        </xdr:nvCxnSpPr>
-        <xdr:spPr>
-          <a:xfrm flipH="1" flipV="1">
-            <a:off x="7532959" y="7663164"/>
-            <a:ext cx="591059" cy="0"/>
-          </a:xfrm>
-          <a:prstGeom prst="straightConnector1">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
-            <a:headEnd type="triangle"/>
-            <a:tailEnd type="triangle"/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-      </xdr:cxnSp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="66" name="TextBox 65">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5E52E92-580C-420E-8836-21C3EE3855D7}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7768849" y="7403669"/>
-            <a:ext cx="2051652" cy="264560"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="tx1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-            <a:spAutoFit/>
-          </a:bodyPr>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1100">
-                <a:solidFill>
-                  <a:srgbClr val="00B050"/>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Range of allowed random values</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1914,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,50 +1670,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB89FDF4-C5C2-405B-8802-1B03DEB1F621}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
+      <c r="A2" t="str">
+        <f>Inputs!A19</f>
+        <v>D</v>
       </c>
       <c r="D2" t="str">
-        <f>IF(C2="Strongly",10,(IF(C2="Weakly",30,"")))</f>
+        <f>IF(C2="Strongly Positive",0.9,IF(C2="Weakly Positive",0.6,IF(C2="Strongly Negative",-0.9,IF(C2="Weakly Negative",-0.6,""))))</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
+      <c r="A3" t="str">
+        <f>Inputs!A20</f>
+        <v>t</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D27" si="0">IF(C3="Strongly",10,(IF(C3="Weakly",30,"")))</f>
+        <f t="shared" ref="D3:D27" si="0">IF(C3="Strongly Positive",0.9,IF(C3="Weakly Positive",0.6,IF(C3="Strongly Negative",-0.9,IF(C3="Weakly Negative",-0.6,""))))</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
+      <c r="A4" t="str">
+        <f>Inputs!A21</f>
+        <v>W_empty</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -2805,8 +1727,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
+      <c r="A5" t="str">
+        <f>Inputs!A22</f>
+        <v>W_hydro</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -2814,8 +1737,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
+      <c r="A6" t="str">
+        <f>Inputs!A23</f>
+        <v>W_op</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -2823,8 +1747,9 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
+      <c r="A7" t="str">
+        <f>Inputs!A24</f>
+        <v>alpha</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -2832,8 +1757,9 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>98</v>
+      <c r="A8" t="str">
+        <f>Inputs!A25</f>
+        <v>EI</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -2841,8 +1767,9 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
+      <c r="A9" t="str">
+        <f>Inputs!A26</f>
+        <v>T0</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -2850,8 +1777,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
+      <c r="A10" t="str">
+        <f>Inputs!A27</f>
+        <v>t_aslaid</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2859,8 +1787,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
+      <c r="A11" t="str">
+        <f>Inputs!A28</f>
+        <v>t_hydro</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -2868,8 +1797,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
+      <c r="A12" t="str">
+        <f>Inputs!A29</f>
+        <v>t_preop</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -2877,8 +1807,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>45</v>
+      <c r="A13" t="str">
+        <f>Inputs!A30</f>
+        <v>su_mudline</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -2887,53 +1818,57 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>47</v>
+      <c r="A14" t="str">
+        <f>Inputs!A31</f>
+        <v>su_inv</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>73</v>
+      <c r="A15" t="str">
+        <f>Inputs!A32</f>
+        <v>delta_su</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>48</v>
+      <c r="A16" t="str">
+        <f>Inputs!A33</f>
+        <v>gamma_sub</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>49</v>
+      <c r="A17" t="str">
+        <f>Inputs!A34</f>
+        <v>pipelay_St</v>
       </c>
       <c r="B17" t="s">
         <v>45</v>
@@ -2943,12 +1878,13 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>50</v>
+      <c r="A18" t="str">
+        <f>Inputs!A35</f>
+        <v>lateral_St</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
@@ -2958,57 +1894,49 @@
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="A19" t="str">
+        <f>Inputs!A36</f>
+        <v>cv</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>52</v>
+      <c r="A20" t="str">
+        <f>Inputs!A37</f>
+        <v>SHANSEP_S</v>
       </c>
       <c r="B20" t="s">
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="A21" t="str">
+        <f>Inputs!A38</f>
+        <v>SHANSEP_m</v>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(C21="Strongly Positive",0.9,IF(C21="Weakly Positive",0.6,IF(C21="Strongly Negative",-0.9,IF(C21="Weakly Negative",-0.6,""))))</f>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>54</v>
+      <c r="A22" t="str">
+        <f>Inputs!A39</f>
+        <v>ka</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -3016,8 +1944,9 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>55</v>
+      <c r="A23" t="str">
+        <f>Inputs!A40</f>
+        <v>kp</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -3025,68 +1954,66 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>56</v>
+      <c r="A24" t="str">
+        <f>Inputs!A41</f>
+        <v>phi</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>57</v>
+      <c r="A25" t="str">
+        <f>Inputs!A42</f>
+        <v>int_SHANSEP_S</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="A26" t="str">
+        <f>Inputs!A43</f>
+        <v>int_SHANSEP_m</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>93</v>
+      <c r="A27" t="str">
+        <f>Inputs!A44</f>
+        <v>delta</v>
       </c>
       <c r="B27" t="s">
         <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Working on output figures
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACC909F-7DE8-40AD-B68C-322EB2A52732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A73340-4CED-4D06-A5B9-E79D894AF68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB89FDF4-C5C2-405B-8802-1B03DEB1F621}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changing to allow multiple models to be run at a time - still need to resolve an issue this has brought up for Lat_res
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A73340-4CED-4D06-A5B9-E79D894AF68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EF4DD2-A6BA-4306-8931-6CC90821D682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="114">
   <si>
     <t>Input File for Pipe-Soil Interaction Analysis</t>
   </si>
@@ -46,18 +46,12 @@
     <t>Instructions</t>
   </si>
   <si>
-    <t>1. Download code from team GitHub</t>
-  </si>
-  <si>
     <t>3. Populate 'Input' tab of this file</t>
   </si>
   <si>
     <t>2. Save this file and code in the same location on your computer named PSI_Inputs</t>
   </si>
   <si>
-    <t>4. Open Matlab file 'PSI_montecarlo' and press run</t>
-  </si>
-  <si>
     <t>Emb_aslaid_model</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>% as above</t>
   </si>
   <si>
-    <t>% undrained: DNVGL-RP-F114 Model 1 = 0, DNVGL-RP-F114 Model 2/SAFEBUCK = 1, Merifield et al 2008/2009 = 2, drained: DNVGL-RP-F114 Model 1 = 10, DNVGL-RP-F114 Model 2/SAFEBUCK = 11</t>
-  </si>
-  <si>
     <t>% switch for suction at rear of pipe, not allowing = 0, allowing = 1 (relevant for lateral breakout undrained DNVGL-RP-F114 Model 1)</t>
   </si>
   <si>
@@ -313,12 +304,6 @@
     <t>% switch for suction at rear of pipe, not allowing = 0, allowing = 1 (relevant for lateral residual undrained modified method)</t>
   </si>
   <si>
-    <t>% as for above embedment models (relevant for lateral residual undrained modified method and drained DNVGL-RP-F114 Model 1)</t>
-  </si>
-  <si>
-    <t>% undrained: modified DNV = 0 (using instantaneous embedment into undisturbed soil profile then same approach as DNVGL-RP-F114 Lat Brk UD Model 1), DNVGL-RP-F114/SAFEBUCK = 1, modified Merifield = 2 (using instantaneous embedment into undisturbed soil profile then same approach as Merifield et al 2008/2009 Lat Brk UD Model), drained: DNVGL-RP-F114 Model 1 = 10, DNVGL-RP-F114 Model 2/SAFEBUCK = 11</t>
-  </si>
-  <si>
     <t>delta</t>
   </si>
   <si>
@@ -368,6 +353,33 @@
   </si>
   <si>
     <t>Base Variable</t>
+  </si>
+  <si>
+    <t>4. Open Python file 'PSI_montecarlo' and press run</t>
+  </si>
+  <si>
+    <t>1. Download code from GitHub</t>
+  </si>
+  <si>
+    <t>% undrained: modified DNV = 0, DNVGL-RP-F114/SAFEBUCK = 1, Generalised FE Envelope = 2; drained: DNVGL-RP-F114 Model 1 = 10, DNVGL-RP-F114 Model 2/SAFEBUCK = 11</t>
+  </si>
+  <si>
+    <t>% undrained: DNVGL-RP-F114 Model 1 = 0, DNVGL-RP-F114 Model 2/SAFEBUCK = 1, Generalised FE Envelope = 2; drained: DNVGL-RP-F114 Model 1 = 10, DNVGL-RP-F114 Model 2/SAFEBUCK = 11</t>
+  </si>
+  <si>
+    <t>% undrained: Embeding into Undisturbed Material DNVGL-RP-F114 Model 1 = 0, Embeding into Undisturbed Material DNVGL-RP-F114 Model 2/SAFEBUCK = 1, Horizontal Point on Generalised FE Envelope = 2; drained: Embeding into Undisturbed Material DNVGL-RP-F114 = 10</t>
+  </si>
+  <si>
+    <t>Lat_brk_weighting</t>
+  </si>
+  <si>
+    <t>% Min and Max weighting applied to Generalised FE Lat_brk result if used in conjunction with another Lat_brk Model; applied based on embedment and where accuracy of other models is expected to be lower</t>
+  </si>
+  <si>
+    <t>Lat_res_weighting</t>
+  </si>
+  <si>
+    <t>% Min and Max weighting applied to Generalised FE Lat_res result if used in conjunction with another Lat_res Model; applied based on embedment and where accuracy of other models is expected to be lower</t>
   </si>
 </sst>
 </file>
@@ -746,7 +758,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,62 +775,62 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -828,10 +840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,805 +854,848 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>10000</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="D12">
-        <v>100</v>
-      </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" t="s">
-        <v>100</v>
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0.32990000000000003</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0.32990000000000003</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.32990000000000003</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="2">
-        <v>2.6599999999999999E-2</v>
-      </c>
-      <c r="C20" s="2">
-        <v>2.6599999999999999E-2</v>
-      </c>
-      <c r="D20" s="2">
-        <v>2.6599999999999999E-2</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>0.89749999999999996</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="C21" s="2">
-        <v>0.89749999999999996</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="D21" s="2">
-        <v>0.89749999999999996</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" t="s">
         <v>75</v>
-      </c>
-      <c r="H21" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2">
-        <v>1.5022</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="C22" s="2">
-        <v>1.5022</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="D22" s="2">
-        <v>1.5022</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H22" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>0.95650000000000002</v>
+        <v>0.89749999999999996</v>
       </c>
       <c r="C23" s="2">
-        <v>1.0155000000000001</v>
+        <v>0.89749999999999996</v>
       </c>
       <c r="D23" s="2">
-        <v>1.0745</v>
-      </c>
-      <c r="E23" s="2">
         <v>0.89749999999999996</v>
       </c>
+      <c r="E23" s="2"/>
       <c r="F23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="H23" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E24" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.5022</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.5022</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.5022</v>
+      </c>
+      <c r="E24" s="2"/>
       <c r="F24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H24" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25">
-        <v>61675</v>
-      </c>
-      <c r="C25">
-        <v>61675</v>
-      </c>
-      <c r="D25">
-        <v>61675</v>
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1.0155000000000001</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1.0745</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.89749999999999996</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>95</v>
+      </c>
+      <c r="G25" t="s">
+        <v>96</v>
       </c>
       <c r="H25" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26">
-        <v>27</v>
-      </c>
-      <c r="C26">
-        <v>100</v>
-      </c>
-      <c r="D26">
-        <v>236</v>
-      </c>
-      <c r="E26">
-        <v>10</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="4"/>
       <c r="F26" t="s">
-        <v>100</v>
-      </c>
-      <c r="G26" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H26" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="2">
+        <v>93</v>
+      </c>
+      <c r="B27">
+        <v>61675</v>
+      </c>
+      <c r="C27">
+        <v>61675</v>
+      </c>
+      <c r="D27">
+        <v>61675</v>
+      </c>
+      <c r="F27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>236</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" t="s">
+        <v>97</v>
+      </c>
+      <c r="H28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C29" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D29" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" t="s">
-        <v>75</v>
-      </c>
-      <c r="H27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="2">
+      <c r="E29" s="2"/>
+      <c r="F29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2">
         <f>1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C30" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D30" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C29" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D29" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" t="s">
-        <v>75</v>
-      </c>
-      <c r="H29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="3">
-        <v>0</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="D30" s="3">
-        <v>3.57</v>
-      </c>
-      <c r="E30" s="3">
-        <v>0</v>
-      </c>
+      <c r="E30" s="2"/>
       <c r="F30" t="s">
-        <v>100</v>
-      </c>
-      <c r="G30" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H30" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1.33</v>
-      </c>
-      <c r="C31" s="3">
-        <v>4.84</v>
-      </c>
-      <c r="D31" s="3">
-        <v>14.29</v>
-      </c>
-      <c r="E31" s="3">
-        <v>0</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B31" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D31" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E31" s="2"/>
       <c r="F31" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H31" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B32" s="3">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="C32" s="3">
-        <v>3</v>
+        <v>0.35</v>
       </c>
       <c r="D32" s="3">
-        <v>7.72</v>
+        <v>3.57</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G32" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H32" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B33" s="3">
-        <v>3.04</v>
+        <v>1.33</v>
       </c>
       <c r="C33" s="3">
-        <v>4.2</v>
+        <v>4.84</v>
       </c>
       <c r="D33" s="3">
-        <v>6.96</v>
+        <v>14.29</v>
       </c>
       <c r="E33" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H33" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="B34" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="C34" s="3">
         <v>3</v>
       </c>
-      <c r="C34" s="3">
-        <v>5</v>
-      </c>
       <c r="D34" s="3">
-        <v>7</v>
-      </c>
-      <c r="E34" s="3"/>
+        <v>7.72</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
       <c r="F34" t="s">
-        <v>75</v>
+        <v>95</v>
+      </c>
+      <c r="G34" t="s">
+        <v>97</v>
       </c>
       <c r="H34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B35" s="3">
-        <v>1.5</v>
+        <v>3.04</v>
       </c>
       <c r="C35" s="3">
-        <v>4.33</v>
+        <v>4.2</v>
       </c>
       <c r="D35" s="3">
-        <v>8.33</v>
+        <v>6.96</v>
       </c>
       <c r="E35" s="3">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36">
-        <v>0.44</v>
-      </c>
-      <c r="C36">
-        <v>17.73</v>
-      </c>
-      <c r="D36">
-        <v>503.82</v>
-      </c>
-      <c r="E36" s="3">
-        <v>0</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B36" s="3">
+        <v>3</v>
+      </c>
+      <c r="C36" s="3">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3">
+        <v>7</v>
+      </c>
+      <c r="E36" s="3"/>
       <c r="F36" t="s">
-        <v>100</v>
-      </c>
-      <c r="G36" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H36" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="C37" s="4">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="D37" s="4">
-        <v>0.35</v>
+        <v>47</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4.33</v>
+      </c>
+      <c r="D37" s="3">
+        <v>8.33</v>
       </c>
       <c r="E37" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G37" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H37" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C38" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E38" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="B38">
+        <v>0.44</v>
+      </c>
+      <c r="C38">
+        <v>17.73</v>
+      </c>
+      <c r="D38">
+        <v>503.82</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
       <c r="F38" t="s">
-        <v>75</v>
+        <v>95</v>
+      </c>
+      <c r="G38" t="s">
+        <v>97</v>
       </c>
       <c r="H38" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B39" s="4">
-        <v>2</v>
+        <v>0.22</v>
       </c>
       <c r="C39" s="4">
-        <v>2.25</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D39" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="E39" s="4"/>
+        <v>0.35</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
       <c r="F39" t="s">
-        <v>75</v>
+        <v>95</v>
+      </c>
+      <c r="G39" t="s">
+        <v>96</v>
       </c>
       <c r="H39" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B40" s="4">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="C40" s="4">
-        <v>2.25</v>
+        <v>0.4</v>
       </c>
       <c r="D40" s="4">
-        <v>2.5</v>
+        <v>0.4</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H40" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41">
-        <v>24</v>
-      </c>
-      <c r="C41">
-        <v>30</v>
-      </c>
-      <c r="D41">
-        <v>42</v>
-      </c>
-      <c r="E41" s="3">
-        <v>0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="D41" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E41" s="4"/>
       <c r="F41" t="s">
-        <v>100</v>
-      </c>
-      <c r="G41" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="H41" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B42" s="4">
-        <v>0.22</v>
+        <v>2</v>
       </c>
       <c r="C42" s="4">
-        <v>0.28499999999999998</v>
+        <v>2.25</v>
       </c>
       <c r="D42" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="E42" s="3">
-        <v>0</v>
-      </c>
+        <v>2.5</v>
+      </c>
+      <c r="E42" s="4"/>
       <c r="F42" t="s">
-        <v>100</v>
-      </c>
-      <c r="G42" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="H42" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="C43" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D43" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E43" s="4"/>
+        <v>53</v>
+      </c>
+      <c r="B43">
+        <v>24</v>
+      </c>
+      <c r="C43">
+        <v>30</v>
+      </c>
+      <c r="D43">
+        <v>42</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0</v>
+      </c>
       <c r="F43" t="s">
-        <v>75</v>
+        <v>95</v>
+      </c>
+      <c r="G43" t="s">
+        <v>97</v>
       </c>
       <c r="H43" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>93</v>
-      </c>
-      <c r="B44" s="3">
-        <v>26.6</v>
-      </c>
-      <c r="C44" s="3">
-        <v>34.6</v>
+        <v>54</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="C44" s="4">
+        <v>0.28499999999999998</v>
       </c>
       <c r="D44" s="4">
-        <v>41.3</v>
+        <v>0.35</v>
       </c>
       <c r="E44" s="3">
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G44" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H44" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" t="s">
+        <v>72</v>
+      </c>
+      <c r="H45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="3">
+        <v>26.6</v>
+      </c>
+      <c r="C46" s="3">
+        <v>34.6</v>
+      </c>
+      <c r="D46" s="4">
+        <v>41.3</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>95</v>
+      </c>
+      <c r="G46" t="s">
+        <v>96</v>
+      </c>
+      <c r="H46" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1652,13 +1707,13 @@
           <x14:formula1>
             <xm:f>Intro!$A$13:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>F19:F44</xm:sqref>
+          <xm:sqref>F21:F46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4A6C1404-CBB2-46E4-A208-B5A1886B394C}">
           <x14:formula1>
             <xm:f>Intro!$A$14:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>B15</xm:sqref>
+          <xm:sqref>B17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1670,7 +1725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB89FDF4-C5C2-405B-8802-1B03DEB1F621}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1684,21 +1739,21 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>Inputs!A19</f>
+        <f>Inputs!A21</f>
         <v>D</v>
       </c>
       <c r="D2" t="str">
@@ -1708,7 +1763,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>Inputs!A20</f>
+        <f>Inputs!A22</f>
         <v>t</v>
       </c>
       <c r="D3" t="str">
@@ -1718,7 +1773,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>Inputs!A21</f>
+        <f>Inputs!A23</f>
         <v>W_empty</v>
       </c>
       <c r="D4" t="str">
@@ -1728,7 +1783,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>Inputs!A22</f>
+        <f>Inputs!A24</f>
         <v>W_hydro</v>
       </c>
       <c r="D5" t="str">
@@ -1738,7 +1793,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>Inputs!A23</f>
+        <f>Inputs!A25</f>
         <v>W_op</v>
       </c>
       <c r="D6" t="str">
@@ -1748,7 +1803,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>Inputs!A24</f>
+        <f>Inputs!A26</f>
         <v>alpha</v>
       </c>
       <c r="D7" t="str">
@@ -1758,7 +1813,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>Inputs!A25</f>
+        <f>Inputs!A27</f>
         <v>EI</v>
       </c>
       <c r="D8" t="str">
@@ -1768,7 +1823,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>Inputs!A26</f>
+        <f>Inputs!A28</f>
         <v>T0</v>
       </c>
       <c r="D9" t="str">
@@ -1778,7 +1833,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>Inputs!A27</f>
+        <f>Inputs!A29</f>
         <v>t_aslaid</v>
       </c>
       <c r="D10" t="str">
@@ -1788,7 +1843,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>Inputs!A28</f>
+        <f>Inputs!A30</f>
         <v>t_hydro</v>
       </c>
       <c r="D11" t="str">
@@ -1798,7 +1853,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>Inputs!A29</f>
+        <f>Inputs!A31</f>
         <v>t_preop</v>
       </c>
       <c r="D12" t="str">
@@ -1808,7 +1863,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>Inputs!A30</f>
+        <f>Inputs!A32</f>
         <v>su_mudline</v>
       </c>
       <c r="D13" t="str">
@@ -1819,14 +1874,14 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>Inputs!A31</f>
+        <f>Inputs!A33</f>
         <v>su_inv</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -1835,14 +1890,14 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>Inputs!A32</f>
+        <f>Inputs!A34</f>
         <v>delta_su</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -1851,14 +1906,14 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>Inputs!A33</f>
+        <f>Inputs!A35</f>
         <v>gamma_sub</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -1867,14 +1922,14 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>Inputs!A34</f>
+        <f>Inputs!A36</f>
         <v>pipelay_St</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -1883,14 +1938,14 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>Inputs!A35</f>
+        <f>Inputs!A37</f>
         <v>lateral_St</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -1899,7 +1954,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>Inputs!A36</f>
+        <f>Inputs!A38</f>
         <v>cv</v>
       </c>
       <c r="D19" t="str">
@@ -1909,14 +1964,14 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>Inputs!A37</f>
+        <f>Inputs!A39</f>
         <v>SHANSEP_S</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -1925,7 +1980,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>Inputs!A38</f>
+        <f>Inputs!A40</f>
         <v>SHANSEP_m</v>
       </c>
       <c r="D21" t="str">
@@ -1935,7 +1990,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>Inputs!A39</f>
+        <f>Inputs!A41</f>
         <v>ka</v>
       </c>
       <c r="D22" t="str">
@@ -1945,7 +2000,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>Inputs!A40</f>
+        <f>Inputs!A42</f>
         <v>kp</v>
       </c>
       <c r="D23" t="str">
@@ -1955,14 +2010,14 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>Inputs!A41</f>
+        <f>Inputs!A43</f>
         <v>phi</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -1971,14 +2026,14 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>Inputs!A42</f>
+        <f>Inputs!A44</f>
         <v>int_SHANSEP_S</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -1987,7 +2042,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>Inputs!A43</f>
+        <f>Inputs!A45</f>
         <v>int_SHANSEP_m</v>
       </c>
       <c r="D26" t="str">
@@ -1997,14 +2052,14 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>Inputs!A44</f>
+        <f>Inputs!A46</f>
         <v>delta</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Changing residual embedment calculation method and some troubleshooting on the UD method weighting calcs
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EF4DD2-A6BA-4306-8931-6CC90821D682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801A3DAD-0E1F-4C50-AD35-1A962725E203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
   <si>
     <t>Input File for Pipe-Soil Interaction Analysis</t>
   </si>
@@ -326,12 +326,6 @@
   </si>
   <si>
     <t>Automated Fit</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>LN</t>
   </si>
   <si>
     <t>Min Value</t>
@@ -775,7 +769,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -790,7 +784,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -840,10 +834,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +898,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -920,7 +914,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B7">
         <v>60</v>
@@ -929,7 +923,7 @@
         <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -946,7 +940,7 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -962,7 +956,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B10">
         <v>60</v>
@@ -971,7 +965,7 @@
         <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -979,10 +973,10 @@
         <v>86</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1049,7 +1043,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1060,12 +1054,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>92</v>
       </c>
@@ -1079,14 +1073,14 @@
         <v>77</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1103,11 +1097,11 @@
       <c r="F21" t="s">
         <v>72</v>
       </c>
-      <c r="H21" t="s">
+      <c r="G21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -1124,11 +1118,11 @@
       <c r="F22" t="s">
         <v>72</v>
       </c>
-      <c r="H22" t="s">
+      <c r="G22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1145,11 +1139,11 @@
       <c r="F23" t="s">
         <v>72</v>
       </c>
-      <c r="H23" t="s">
+      <c r="G23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1166,11 +1160,11 @@
       <c r="F24" t="s">
         <v>72</v>
       </c>
-      <c r="H24" t="s">
+      <c r="G24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1190,13 +1184,10 @@
         <v>95</v>
       </c>
       <c r="G25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1213,11 +1204,11 @@
       <c r="F26" t="s">
         <v>72</v>
       </c>
-      <c r="H26" t="s">
+      <c r="G26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -1233,11 +1224,11 @@
       <c r="F27" t="s">
         <v>72</v>
       </c>
-      <c r="H27" t="s">
+      <c r="G27" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1257,13 +1248,10 @@
         <v>95</v>
       </c>
       <c r="G28" t="s">
-        <v>97</v>
-      </c>
-      <c r="H28" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1281,11 +1269,11 @@
       <c r="F29" t="s">
         <v>72</v>
       </c>
-      <c r="H29" t="s">
+      <c r="G29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1303,11 +1291,11 @@
       <c r="F30" t="s">
         <v>72</v>
       </c>
-      <c r="H30" t="s">
+      <c r="G30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1324,11 +1312,11 @@
       <c r="F31" t="s">
         <v>72</v>
       </c>
-      <c r="H31" t="s">
+      <c r="G31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1348,13 +1336,10 @@
         <v>95</v>
       </c>
       <c r="G32" t="s">
-        <v>97</v>
-      </c>
-      <c r="H32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1374,13 +1359,10 @@
         <v>95</v>
       </c>
       <c r="G33" t="s">
-        <v>97</v>
-      </c>
-      <c r="H33" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -1400,13 +1382,10 @@
         <v>95</v>
       </c>
       <c r="G34" t="s">
-        <v>97</v>
-      </c>
-      <c r="H34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1426,13 +1405,10 @@
         <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>97</v>
-      </c>
-      <c r="H35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1449,22 +1425,22 @@
       <c r="F36" t="s">
         <v>72</v>
       </c>
-      <c r="H36" t="s">
+      <c r="G36" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
         <v>1.5</v>
       </c>
-      <c r="C37" s="3">
-        <v>4.33</v>
-      </c>
       <c r="D37" s="3">
-        <v>8.33</v>
+        <v>2</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
@@ -1473,13 +1449,10 @@
         <v>95</v>
       </c>
       <c r="G37" t="s">
-        <v>97</v>
-      </c>
-      <c r="H37" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -1499,13 +1472,10 @@
         <v>95</v>
       </c>
       <c r="G38" t="s">
-        <v>97</v>
-      </c>
-      <c r="H38" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1525,13 +1495,10 @@
         <v>95</v>
       </c>
       <c r="G39" t="s">
-        <v>96</v>
-      </c>
-      <c r="H39" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -1548,11 +1515,11 @@
       <c r="F40" t="s">
         <v>72</v>
       </c>
-      <c r="H40" t="s">
+      <c r="G40" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -1569,11 +1536,11 @@
       <c r="F41" t="s">
         <v>72</v>
       </c>
-      <c r="H41" t="s">
+      <c r="G41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -1590,11 +1557,11 @@
       <c r="F42" t="s">
         <v>72</v>
       </c>
-      <c r="H42" t="s">
+      <c r="G42" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -1614,13 +1581,10 @@
         <v>95</v>
       </c>
       <c r="G43" t="s">
-        <v>97</v>
-      </c>
-      <c r="H43" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -1640,13 +1604,10 @@
         <v>95</v>
       </c>
       <c r="G44" t="s">
-        <v>96</v>
-      </c>
-      <c r="H44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -1663,11 +1624,11 @@
       <c r="F45" t="s">
         <v>72</v>
       </c>
-      <c r="H45" t="s">
+      <c r="G45" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -1687,13 +1648,10 @@
         <v>95</v>
       </c>
       <c r="G46" t="s">
-        <v>96</v>
-      </c>
-      <c r="H46" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
     </row>
@@ -1742,13 +1700,13 @@
         <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1881,7 +1839,7 @@
         <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -1897,7 +1855,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -1913,7 +1871,7 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -1929,7 +1887,7 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -1945,7 +1903,7 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -1971,7 +1929,7 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -2017,7 +1975,7 @@
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -2033,7 +1991,7 @@
         <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -2059,7 +2017,7 @@
         <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Changes to weighting to account for where different methods are more reliable, and addition of model factor to the post-processing for figures and 5, 50, 95% (note saved data is without model factor so it isn't accidentally applied repeatedly
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801A3DAD-0E1F-4C50-AD35-1A962725E203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241122DD-720E-4608-BB35-981DD12D3EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="114">
   <si>
     <t>Input File for Pipe-Soil Interaction Analysis</t>
   </si>
@@ -374,6 +374,12 @@
   </si>
   <si>
     <t>% Min and Max weighting applied to Generalised FE Lat_res result if used in conjunction with another Lat_res Model; applied based on embedment and where accuracy of other models is expected to be lower</t>
+  </si>
+  <si>
+    <t>Model_fct</t>
+  </si>
+  <si>
+    <t>% factor applied to all results to arbitrarily account for additional uncertainty by increaisng the bounds; applied linearly for each result where min/1.2 and max*1.2; MEAN WILL BE AFFECTED UNLESS IT IS HALF-WAY BETWEEN MIN AND MAX IN MAGNITUDE</t>
   </si>
 </sst>
 </file>
@@ -834,10 +840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,303 +1060,291 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18">
+        <v>1.2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0.32990000000000003</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0.32990000000000003</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.32990000000000003</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" t="s">
-        <v>75</v>
-      </c>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>2.6599999999999999E-2</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="C22" s="2">
-        <v>2.6599999999999999E-2</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="D22" s="2">
-        <v>2.6599999999999999E-2</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" t="s">
         <v>72</v>
       </c>
       <c r="G22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B23" s="2">
-        <v>0.89749999999999996</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="C23" s="2">
-        <v>0.89749999999999996</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="D23" s="2">
-        <v>0.89749999999999996</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s">
         <v>72</v>
       </c>
       <c r="G23" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>1.5022</v>
+        <v>0.89749999999999996</v>
       </c>
       <c r="C24" s="2">
-        <v>1.5022</v>
+        <v>0.89749999999999996</v>
       </c>
       <c r="D24" s="2">
-        <v>1.5022</v>
+        <v>0.89749999999999996</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s">
         <v>72</v>
       </c>
       <c r="G24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>0.95650000000000002</v>
+        <v>1.5022</v>
       </c>
       <c r="C25" s="2">
-        <v>1.0155000000000001</v>
+        <v>1.5022</v>
       </c>
       <c r="D25" s="2">
-        <v>1.0745</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0.89749999999999996</v>
-      </c>
+        <v>1.5022</v>
+      </c>
+      <c r="E25" s="2"/>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C26" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E26" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1.0155000000000001</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.0745</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.89749999999999996</v>
+      </c>
       <c r="F26" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="G26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27">
-        <v>61675</v>
-      </c>
-      <c r="C27">
-        <v>61675</v>
-      </c>
-      <c r="D27">
-        <v>61675</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="4"/>
       <c r="F27" t="s">
         <v>72</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>61675</v>
       </c>
       <c r="C28">
-        <v>100</v>
+        <v>61675</v>
       </c>
       <c r="D28">
-        <v>236</v>
-      </c>
-      <c r="E28">
-        <v>10</v>
+        <v>61675</v>
       </c>
       <c r="F28" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G28" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
         <v>27</v>
       </c>
-      <c r="B29" s="2">
+      <c r="C29">
+        <v>100</v>
+      </c>
+      <c r="D29">
+        <v>236</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
+      </c>
+      <c r="G29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="2">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C30" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D30" s="2">
         <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="2">
-        <f>1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C30" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D30" s="2">
-        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" t="s">
         <v>72</v>
       </c>
       <c r="G30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="2">
-        <v>8.3333333333333329E-2</v>
+        <f>1/24</f>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C31" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D31" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s">
         <v>72</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="3">
-        <v>0</v>
-      </c>
-      <c r="C32" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="D32" s="3">
-        <v>3.57</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B32" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C32" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D32" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E32" s="2"/>
       <c r="F32" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G32" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B33" s="3">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="C33" s="3">
-        <v>4.84</v>
+        <v>0.35</v>
       </c>
       <c r="D33" s="3">
-        <v>14.29</v>
+        <v>3.57</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
@@ -1359,21 +1353,21 @@
         <v>95</v>
       </c>
       <c r="G33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B34" s="3">
         <v>1.33</v>
       </c>
       <c r="C34" s="3">
-        <v>3</v>
+        <v>4.84</v>
       </c>
       <c r="D34" s="3">
-        <v>7.72</v>
+        <v>14.29</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
@@ -1382,111 +1376,111 @@
         <v>95</v>
       </c>
       <c r="G34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B35" s="3">
-        <v>3.04</v>
+        <v>1.33</v>
       </c>
       <c r="C35" s="3">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="D35" s="3">
-        <v>6.96</v>
+        <v>7.72</v>
       </c>
       <c r="E35" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="s">
         <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="3">
-        <v>3</v>
+        <v>3.04</v>
       </c>
       <c r="C36" s="3">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="D36" s="3">
-        <v>7</v>
-      </c>
-      <c r="E36" s="3"/>
+        <v>6.96</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
       <c r="F36" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="G36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B37" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C37" s="3">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="D37" s="3">
-        <v>2</v>
-      </c>
-      <c r="E37" s="3">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E37" s="3"/>
       <c r="F37" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38">
-        <v>0.44</v>
-      </c>
-      <c r="C38">
-        <v>17.73</v>
-      </c>
-      <c r="D38">
-        <v>503.82</v>
+        <v>47</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D38" s="3">
+        <v>2</v>
       </c>
       <c r="E38" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
         <v>95</v>
       </c>
       <c r="G38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="C39" s="4">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0.35</v>
+        <v>48</v>
+      </c>
+      <c r="B39">
+        <v>0.44</v>
+      </c>
+      <c r="C39">
+        <v>17.73</v>
+      </c>
+      <c r="D39">
+        <v>503.82</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
@@ -1495,54 +1489,56 @@
         <v>95</v>
       </c>
       <c r="G39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="4">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="C40" s="4">
-        <v>0.4</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D40" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E40" s="4"/>
+        <v>0.35</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
       <c r="F40" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="G40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" s="4">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="C41" s="4">
-        <v>2.25</v>
+        <v>0.4</v>
       </c>
       <c r="D41" s="4">
-        <v>2.5</v>
+        <v>0.4</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" t="s">
         <v>72</v>
       </c>
       <c r="G41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" s="4">
         <v>2</v>
@@ -1558,44 +1554,42 @@
         <v>72</v>
       </c>
       <c r="G42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43">
-        <v>24</v>
-      </c>
-      <c r="C43">
-        <v>30</v>
-      </c>
-      <c r="D43">
-        <v>42</v>
-      </c>
-      <c r="E43" s="3">
-        <v>0</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B43" s="4">
+        <v>2</v>
+      </c>
+      <c r="C43" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="D43" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E43" s="4"/>
       <c r="F43" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="C44" s="4">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="D44" s="4">
-        <v>0.35</v>
+        <v>53</v>
+      </c>
+      <c r="B44">
+        <v>24</v>
+      </c>
+      <c r="C44">
+        <v>30</v>
+      </c>
+      <c r="D44">
+        <v>42</v>
       </c>
       <c r="E44" s="3">
         <v>0</v>
@@ -1604,56 +1598,79 @@
         <v>95</v>
       </c>
       <c r="G44" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" s="4">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="C45" s="4">
-        <v>0.4</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D45" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E45" s="4"/>
+        <v>0.35</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0</v>
+      </c>
       <c r="F45" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="G45" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" t="s">
+        <v>72</v>
+      </c>
+      <c r="G46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B47" s="3">
         <v>26.6</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C47" s="3">
         <v>34.6</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D47" s="4">
         <v>41.3</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E47" s="3">
         <v>0</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F47" t="s">
         <v>95</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1665,7 +1682,7 @@
           <x14:formula1>
             <xm:f>Intro!$A$13:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>F21:F46</xm:sqref>
+          <xm:sqref>F22:F47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4A6C1404-CBB2-46E4-A208-B5A1886B394C}">
           <x14:formula1>
@@ -1711,7 +1728,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>Inputs!A21</f>
+        <f>Inputs!A22</f>
         <v>D</v>
       </c>
       <c r="D2" t="str">
@@ -1721,7 +1738,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>Inputs!A22</f>
+        <f>Inputs!A23</f>
         <v>t</v>
       </c>
       <c r="D3" t="str">
@@ -1731,7 +1748,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>Inputs!A23</f>
+        <f>Inputs!A24</f>
         <v>W_empty</v>
       </c>
       <c r="D4" t="str">
@@ -1741,7 +1758,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>Inputs!A24</f>
+        <f>Inputs!A25</f>
         <v>W_hydro</v>
       </c>
       <c r="D5" t="str">
@@ -1751,7 +1768,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>Inputs!A25</f>
+        <f>Inputs!A26</f>
         <v>W_op</v>
       </c>
       <c r="D6" t="str">
@@ -1761,7 +1778,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>Inputs!A26</f>
+        <f>Inputs!A27</f>
         <v>alpha</v>
       </c>
       <c r="D7" t="str">
@@ -1771,7 +1788,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>Inputs!A27</f>
+        <f>Inputs!A28</f>
         <v>EI</v>
       </c>
       <c r="D8" t="str">
@@ -1781,7 +1798,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>Inputs!A28</f>
+        <f>Inputs!A29</f>
         <v>T0</v>
       </c>
       <c r="D9" t="str">
@@ -1791,7 +1808,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>Inputs!A29</f>
+        <f>Inputs!A30</f>
         <v>t_aslaid</v>
       </c>
       <c r="D10" t="str">
@@ -1801,7 +1818,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>Inputs!A30</f>
+        <f>Inputs!A31</f>
         <v>t_hydro</v>
       </c>
       <c r="D11" t="str">
@@ -1811,7 +1828,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>Inputs!A31</f>
+        <f>Inputs!A32</f>
         <v>t_preop</v>
       </c>
       <c r="D12" t="str">
@@ -1821,7 +1838,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>Inputs!A32</f>
+        <f>Inputs!A33</f>
         <v>su_mudline</v>
       </c>
       <c r="D13" t="str">
@@ -1832,7 +1849,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>Inputs!A33</f>
+        <f>Inputs!A34</f>
         <v>su_inv</v>
       </c>
       <c r="B14" t="s">
@@ -1848,7 +1865,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>Inputs!A34</f>
+        <f>Inputs!A35</f>
         <v>delta_su</v>
       </c>
       <c r="B15" t="s">
@@ -1864,7 +1881,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>Inputs!A35</f>
+        <f>Inputs!A36</f>
         <v>gamma_sub</v>
       </c>
       <c r="B16" t="s">
@@ -1880,7 +1897,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>Inputs!A36</f>
+        <f>Inputs!A37</f>
         <v>pipelay_St</v>
       </c>
       <c r="B17" t="s">
@@ -1896,7 +1913,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>Inputs!A37</f>
+        <f>Inputs!A38</f>
         <v>lateral_St</v>
       </c>
       <c r="B18" t="s">
@@ -1912,7 +1929,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>Inputs!A38</f>
+        <f>Inputs!A39</f>
         <v>cv</v>
       </c>
       <c r="D19" t="str">
@@ -1922,7 +1939,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>Inputs!A39</f>
+        <f>Inputs!A40</f>
         <v>SHANSEP_S</v>
       </c>
       <c r="B20" t="s">
@@ -1938,7 +1955,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>Inputs!A40</f>
+        <f>Inputs!A41</f>
         <v>SHANSEP_m</v>
       </c>
       <c r="D21" t="str">
@@ -1948,7 +1965,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>Inputs!A41</f>
+        <f>Inputs!A42</f>
         <v>ka</v>
       </c>
       <c r="D22" t="str">
@@ -1958,7 +1975,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>Inputs!A42</f>
+        <f>Inputs!A43</f>
         <v>kp</v>
       </c>
       <c r="D23" t="str">
@@ -1968,7 +1985,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>Inputs!A43</f>
+        <f>Inputs!A44</f>
         <v>phi</v>
       </c>
       <c r="B24" t="s">
@@ -1984,7 +2001,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>Inputs!A44</f>
+        <f>Inputs!A45</f>
         <v>int_SHANSEP_S</v>
       </c>
       <c r="B25" t="s">
@@ -2000,7 +2017,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>Inputs!A45</f>
+        <f>Inputs!A46</f>
         <v>int_SHANSEP_m</v>
       </c>
       <c r="D26" t="str">
@@ -2010,7 +2027,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>Inputs!A46</f>
+        <f>Inputs!A47</f>
         <v>delta</v>
       </c>
       <c r="B27" t="s">

</xml_diff>

<commit_message>
Adding cyclic transition from UD to D method
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241122DD-720E-4608-BB35-981DD12D3EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167ACBE4-8D7D-4316-A3DE-9760D256A2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="116">
   <si>
     <t>Input File for Pipe-Soil Interaction Analysis</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Ax_model</t>
   </si>
   <si>
-    <t>Lat_cyc_model</t>
-  </si>
-  <si>
     <t>No_cycles</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>% undrained: SAFEBUCK with rate effects from DNVGL-RP-F114 = 0 (SAFEBUCK chosen over DNV as it directly uses interface strength profile rather than applying alpha factor for roughness and epsilon factor for partial remoulding, but otherwise calculation is the same), drained: DNVGL-RP-F114/SAFEBUCK = 10</t>
   </si>
   <si>
-    <t>% undrained: SAFEBUCK = 0 (not included in DNVGL-RP-F114)</t>
-  </si>
-  <si>
     <t>% number of cycles to model for lateral cyclic resistance calculations</t>
   </si>
   <si>
@@ -380,6 +374,18 @@
   </si>
   <si>
     <t>% factor applied to all results to arbitrarily account for additional uncertainty by increaisng the bounds; applied linearly for each result where min/1.2 and max*1.2; MEAN WILL BE AFFECTED UNLESS IT IS HALF-WAY BETWEEN MIN AND MAX IN MAGNITUDE</t>
+  </si>
+  <si>
+    <t>N50</t>
+  </si>
+  <si>
+    <t>% number of cycles for 50% transition between UD and D; Yan et al. 2014 examples approx. N50 = 2 (N95 = 5) and N50 = 4 (N95 = 18); more examples shown in excel 'Cyclic Curves from Yan 2014'</t>
+  </si>
+  <si>
+    <t>Cyc_model</t>
+  </si>
+  <si>
+    <t>% SAFEBUCK UD Lateral = 0 (not included in DNVGL-RP-F114, no axial option included); White &amp; Cheuk 2008 = 1;  Internal method transitioning from UD to D = 2</t>
   </si>
 </sst>
 </file>
@@ -775,7 +781,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -790,47 +796,47 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -840,10 +846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,18 +860,18 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>10000</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -876,7 +882,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -887,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -904,7 +910,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -915,12 +921,12 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7">
         <v>60</v>
@@ -929,7 +935,7 @@
         <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -946,23 +952,23 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10">
         <v>60</v>
@@ -971,18 +977,18 @@
         <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -996,23 +1002,23 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1024,542 +1030,532 @@
         <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" t="s">
-        <v>95</v>
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <v>0.5</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>112</v>
-      </c>
-      <c r="B18">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19">
         <v>1.2</v>
       </c>
-      <c r="G18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
+      <c r="G19" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>31</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0.32990000000000003</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0.32990000000000003</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.32990000000000003</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="A22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="B23" s="2">
-        <v>2.6599999999999999E-2</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="C23" s="2">
-        <v>2.6599999999999999E-2</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="D23" s="2">
-        <v>2.6599999999999999E-2</v>
+        <v>0.32990000000000003</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B24" s="2">
-        <v>0.89749999999999996</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="C24" s="2">
-        <v>0.89749999999999996</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="D24" s="2">
-        <v>0.89749999999999996</v>
+        <v>2.6599999999999999E-2</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
         <v>72</v>
-      </c>
-      <c r="G24" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" s="2">
-        <v>1.5022</v>
+        <v>0.89749999999999996</v>
       </c>
       <c r="C25" s="2">
-        <v>1.5022</v>
+        <v>0.89749999999999996</v>
       </c>
       <c r="D25" s="2">
-        <v>1.5022</v>
+        <v>0.89749999999999996</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2">
-        <v>0.95650000000000002</v>
+        <v>1.5022</v>
       </c>
       <c r="C26" s="2">
-        <v>1.0155000000000001</v>
+        <v>1.5022</v>
       </c>
       <c r="D26" s="2">
-        <v>1.0745</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.89749999999999996</v>
-      </c>
+        <v>1.5022</v>
+      </c>
+      <c r="E26" s="2"/>
       <c r="F26" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E27" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.95650000000000002</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.0155000000000001</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.0745</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.89749999999999996</v>
+      </c>
       <c r="F27" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="G27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28">
-        <v>61675</v>
-      </c>
-      <c r="C28">
-        <v>61675</v>
-      </c>
-      <c r="D28">
-        <v>61675</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="4"/>
       <c r="F28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="B29">
-        <v>27</v>
+        <v>61675</v>
       </c>
       <c r="C29">
-        <v>100</v>
+        <v>61675</v>
       </c>
       <c r="D29">
-        <v>236</v>
-      </c>
-      <c r="E29">
-        <v>10</v>
+        <v>61675</v>
       </c>
       <c r="F29" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30">
         <v>27</v>
       </c>
-      <c r="B30" s="2">
+      <c r="C30">
+        <v>100</v>
+      </c>
+      <c r="D30">
+        <v>236</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="2">
         <f>1/12</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D31" s="2">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="2">
+      <c r="E31" s="2"/>
+      <c r="F31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2">
         <f>1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C32" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D32" s="2">
         <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" t="s">
-        <v>72</v>
-      </c>
-      <c r="G31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C32" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D32" s="2">
-        <v>8.3333333333333329E-2</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="3">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0.35</v>
-      </c>
-      <c r="D33" s="3">
-        <v>3.57</v>
-      </c>
-      <c r="E33" s="3">
-        <v>0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B33" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C33" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E33" s="2"/>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G33" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B34" s="3">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="C34" s="3">
-        <v>4.84</v>
+        <v>0.35</v>
       </c>
       <c r="D34" s="3">
-        <v>14.29</v>
+        <v>3.57</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="B35" s="3">
         <v>1.33</v>
       </c>
       <c r="C35" s="3">
-        <v>3</v>
+        <v>4.84</v>
       </c>
       <c r="D35" s="3">
-        <v>7.72</v>
+        <v>14.29</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G35" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B36" s="3">
-        <v>3.04</v>
+        <v>1.33</v>
       </c>
       <c r="C36" s="3">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="D36" s="3">
-        <v>6.96</v>
+        <v>7.72</v>
       </c>
       <c r="E36" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G36" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B37" s="3">
-        <v>3</v>
+        <v>3.04</v>
       </c>
       <c r="C37" s="3">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="D37" s="3">
-        <v>7</v>
-      </c>
-      <c r="E37" s="3"/>
+        <v>6.96</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
       <c r="F37" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="G37" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B38" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38" s="3">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="D38" s="3">
-        <v>2</v>
-      </c>
-      <c r="E38" s="3">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E38" s="3"/>
       <c r="F38" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G38" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39">
-        <v>0.44</v>
-      </c>
-      <c r="C39">
-        <v>17.73</v>
-      </c>
-      <c r="D39">
-        <v>503.82</v>
+        <v>45</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D39" s="3">
+        <v>2</v>
       </c>
       <c r="E39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G39" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="C40" s="4">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="D40" s="4">
-        <v>0.35</v>
+        <v>46</v>
+      </c>
+      <c r="B40">
+        <v>0.44</v>
+      </c>
+      <c r="C40">
+        <v>17.73</v>
+      </c>
+      <c r="D40">
+        <v>503.82</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G40" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B41" s="4">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="C41" s="4">
-        <v>0.4</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D41" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E41" s="4"/>
+        <v>0.35</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
       <c r="F41" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="G41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B42" s="4">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="C42" s="4">
-        <v>2.25</v>
+        <v>0.4</v>
       </c>
       <c r="D42" s="4">
-        <v>2.5</v>
+        <v>0.4</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G42" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B43" s="4">
         <v>2</v>
@@ -1572,105 +1568,126 @@
       </c>
       <c r="E43" s="4"/>
       <c r="F43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44">
-        <v>24</v>
-      </c>
-      <c r="C44">
-        <v>30</v>
-      </c>
-      <c r="D44">
-        <v>42</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B44" s="4">
+        <v>2</v>
+      </c>
+      <c r="C44" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="D44" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E44" s="4"/>
       <c r="F44" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G44" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="C45" s="4">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="D45" s="4">
-        <v>0.35</v>
+        <v>51</v>
+      </c>
+      <c r="B45">
+        <v>24</v>
+      </c>
+      <c r="C45">
+        <v>30</v>
+      </c>
+      <c r="D45">
+        <v>42</v>
       </c>
       <c r="E45" s="3">
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G45" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B46" s="4">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="C46" s="4">
-        <v>0.4</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D46" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E46" s="4"/>
+        <v>0.35</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
       <c r="F46" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="G46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" t="s">
+        <v>70</v>
+      </c>
+      <c r="G47" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="3">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="3">
         <v>26.6</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C48" s="3">
         <v>34.6</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D48" s="4">
         <v>41.3</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E48" s="3">
         <v>0</v>
       </c>
-      <c r="F47" t="s">
-        <v>95</v>
-      </c>
-      <c r="G47" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+      <c r="F48" t="s">
+        <v>93</v>
+      </c>
+      <c r="G48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1682,13 +1699,13 @@
           <x14:formula1>
             <xm:f>Intro!$A$13:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>F22:F47</xm:sqref>
+          <xm:sqref>F23:F48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4A6C1404-CBB2-46E4-A208-B5A1886B394C}">
           <x14:formula1>
             <xm:f>Intro!$A$14:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>B17</xm:sqref>
+          <xm:sqref>B18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1714,21 +1731,21 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>Inputs!A22</f>
+        <f>Inputs!A23</f>
         <v>D</v>
       </c>
       <c r="D2" t="str">
@@ -1738,7 +1755,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>Inputs!A23</f>
+        <f>Inputs!A24</f>
         <v>t</v>
       </c>
       <c r="D3" t="str">
@@ -1748,7 +1765,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>Inputs!A24</f>
+        <f>Inputs!A25</f>
         <v>W_empty</v>
       </c>
       <c r="D4" t="str">
@@ -1758,7 +1775,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>Inputs!A25</f>
+        <f>Inputs!A26</f>
         <v>W_hydro</v>
       </c>
       <c r="D5" t="str">
@@ -1768,7 +1785,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>Inputs!A26</f>
+        <f>Inputs!A27</f>
         <v>W_op</v>
       </c>
       <c r="D6" t="str">
@@ -1778,7 +1795,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>Inputs!A27</f>
+        <f>Inputs!A28</f>
         <v>alpha</v>
       </c>
       <c r="D7" t="str">
@@ -1788,7 +1805,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>Inputs!A28</f>
+        <f>Inputs!A29</f>
         <v>EI</v>
       </c>
       <c r="D8" t="str">
@@ -1798,7 +1815,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>Inputs!A29</f>
+        <f>Inputs!A30</f>
         <v>T0</v>
       </c>
       <c r="D9" t="str">
@@ -1808,7 +1825,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>Inputs!A30</f>
+        <f>Inputs!A31</f>
         <v>t_aslaid</v>
       </c>
       <c r="D10" t="str">
@@ -1818,7 +1835,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>Inputs!A31</f>
+        <f>Inputs!A32</f>
         <v>t_hydro</v>
       </c>
       <c r="D11" t="str">
@@ -1828,7 +1845,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>Inputs!A32</f>
+        <f>Inputs!A33</f>
         <v>t_preop</v>
       </c>
       <c r="D12" t="str">
@@ -1838,7 +1855,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>Inputs!A33</f>
+        <f>Inputs!A34</f>
         <v>su_mudline</v>
       </c>
       <c r="D13" t="str">
@@ -1849,14 +1866,14 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>Inputs!A34</f>
+        <f>Inputs!A35</f>
         <v>su_inv</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -1865,14 +1882,14 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>Inputs!A35</f>
+        <f>Inputs!A36</f>
         <v>delta_su</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -1881,14 +1898,14 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>Inputs!A36</f>
+        <f>Inputs!A37</f>
         <v>gamma_sub</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -1897,14 +1914,14 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>Inputs!A37</f>
+        <f>Inputs!A38</f>
         <v>pipelay_St</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -1913,14 +1930,14 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>Inputs!A38</f>
+        <f>Inputs!A39</f>
         <v>lateral_St</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -1929,7 +1946,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>Inputs!A39</f>
+        <f>Inputs!A40</f>
         <v>cv</v>
       </c>
       <c r="D19" t="str">
@@ -1939,14 +1956,14 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>Inputs!A40</f>
+        <f>Inputs!A41</f>
         <v>SHANSEP_S</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -1955,7 +1972,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>Inputs!A41</f>
+        <f>Inputs!A42</f>
         <v>SHANSEP_m</v>
       </c>
       <c r="D21" t="str">
@@ -1965,7 +1982,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>Inputs!A42</f>
+        <f>Inputs!A43</f>
         <v>ka</v>
       </c>
       <c r="D22" t="str">
@@ -1975,7 +1992,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>Inputs!A43</f>
+        <f>Inputs!A44</f>
         <v>kp</v>
       </c>
       <c r="D23" t="str">
@@ -1985,14 +2002,14 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>Inputs!A44</f>
+        <f>Inputs!A45</f>
         <v>phi</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -2001,14 +2018,14 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>Inputs!A45</f>
+        <f>Inputs!A46</f>
         <v>int_SHANSEP_S</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -2017,7 +2034,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>Inputs!A46</f>
+        <f>Inputs!A47</f>
         <v>int_SHANSEP_m</v>
       </c>
       <c r="D26" t="str">
@@ -2027,14 +2044,14 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>Inputs!A47</f>
+        <f>Inputs!A48</f>
         <v>delta</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Updates to output figures
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167ACBE4-8D7D-4316-A3DE-9760D256A2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE6913B-F763-4FF8-BF1D-BDF9DDD39839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -849,7 +849,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor fixes as running code
</commit_message>
<xml_diff>
--- a/PSI_inputs.xlsx
+++ b/PSI_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AUSM504495\Documents\GitHub\WSP_PSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE6913B-F763-4FF8-BF1D-BDF9DDD39839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C47634-20CB-4764-82E1-FC391F7841B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1D4F1EAD-D63C-4463-81B7-10D96C3C5F00}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="118">
   <si>
     <t>Input File for Pipe-Soil Interaction Analysis</t>
   </si>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>% SAFEBUCK UD Lateral = 0 (not included in DNVGL-RP-F114, no axial option included); White &amp; Cheuk 2008 = 1;  Internal method transitioning from UD to D = 2</t>
+  </si>
+  <si>
+    <t>pipelay_Fct</t>
+  </si>
+  <si>
+    <t>% soil-soil: factor applied to phi to account for dynamic effects during pipelay, similar to pipelay_St for undrained</t>
   </si>
 </sst>
 </file>
@@ -440,13 +446,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,10 +853,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A463C4-1722-4182-9BE8-8462E138567F}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,74 +1627,97 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="C46" s="4">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="D46" s="4">
-        <v>0.35</v>
+        <v>116</v>
+      </c>
+      <c r="B46" s="6">
+        <v>10</v>
+      </c>
+      <c r="C46" s="6">
+        <v>50</v>
+      </c>
+      <c r="D46" s="6">
+        <v>100</v>
       </c>
       <c r="E46" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" t="s">
         <v>93</v>
       </c>
       <c r="G46" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="4">
-        <v>0.4</v>
+        <v>0.22</v>
       </c>
       <c r="C47" s="4">
-        <v>0.4</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="D47" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="E47" s="4"/>
+        <v>0.35</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
       <c r="F47" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="G47" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" t="s">
+        <v>70</v>
+      </c>
+      <c r="G48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B49" s="3">
         <v>26.6</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C49" s="3">
         <v>34.6</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D49" s="4">
         <v>41.3</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E49" s="3">
         <v>0</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>93</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1699,7 +1729,7 @@
           <x14:formula1>
             <xm:f>Intro!$A$13:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>F23:F48</xm:sqref>
+          <xm:sqref>F23:F45 F47:F49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4A6C1404-CBB2-46E4-A208-B5A1886B394C}">
           <x14:formula1>
@@ -2018,7 +2048,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>Inputs!A46</f>
+        <f>Inputs!A47</f>
         <v>int_SHANSEP_S</v>
       </c>
       <c r="B25" t="s">
@@ -2034,7 +2064,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>Inputs!A47</f>
+        <f>Inputs!A48</f>
         <v>int_SHANSEP_m</v>
       </c>
       <c r="D26" t="str">
@@ -2044,7 +2074,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>Inputs!A48</f>
+        <f>Inputs!A49</f>
         <v>delta</v>
       </c>
       <c r="B27" t="s">

</xml_diff>